<commit_message>
making get_value function wich allow to get the value of a gave cell, gaving also the file path and the sheet, knowing that there is a default value for the sheet name.
</commit_message>
<xml_diff>
--- a/excel/test1.xlsx
+++ b/excel/test1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\programmation\python\ranked_notes\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F82BAA4-51FC-4D66-8609-3054D0CAA183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180900BF-51D5-4A73-A768-8768418035DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 5" sheetId="5" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>

</xml_diff>

<commit_message>
Making a writing value funcion which allow to write a value or an instruction in a gave cell position on a file for wich the path is gave too
</commit_message>
<xml_diff>
--- a/excel/test1.xlsx
+++ b/excel/test1.xlsx
@@ -1,55 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\programmation\python\ranked_notes\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180900BF-51D5-4A73-A768-8768418035DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75984D36-8ED3-4201-8B63-200D53EDDDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="5" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>code UPHF</t>
-    </r>
+    <t>code UPHF</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note</t>
-    </r>
+    <t>Note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -70,6 +62,12 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF98C379"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -112,27 +110,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="7" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="7" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="15"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,21 +473,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="30" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>22004557</v>
       </c>
@@ -501,7 +503,7 @@
         <v>8.3800000000000008</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>22006418</v>
       </c>
@@ -509,64 +511,76 @@
         <v>10.130000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>22004377</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>14.5</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>22005661</v>
       </c>
       <c r="B5" s="3">
         <v>11.88</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>22003958</v>
       </c>
       <c r="B6" s="3">
         <v>13.38</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="8">
+        <f>SUM(B3:B20)</f>
+        <v>234.04</v>
+      </c>
+      <c r="H6" s="8">
+        <f>SUM(B3:B20)</f>
+        <v>234.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>22007092</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>11.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>22004969</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>22006424</v>
       </c>
       <c r="B9" s="3">
         <v>12.13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>22003983</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>19.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>22005811</v>
       </c>
@@ -574,15 +588,15 @@
         <v>13.38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>22005223</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>12.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>22005894</v>
       </c>
@@ -590,7 +604,7 @@
         <v>9.1300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>22004834</v>
       </c>
@@ -598,7 +612,7 @@
         <v>12.63</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>22006328</v>
       </c>
@@ -606,7 +620,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>22005075</v>
       </c>
@@ -618,7 +632,7 @@
       <c r="A17" s="2">
         <v>22006576</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>10</v>
       </c>
     </row>
@@ -626,7 +640,7 @@
       <c r="A18" s="2">
         <v>22005895</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>12</v>
       </c>
     </row>
@@ -648,5 +662,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>